<commit_message>
Update of Test cases after testing
</commit_message>
<xml_diff>
--- a/Documents/Agile-test-plan-template.xlsx
+++ b/Documents/Agile-test-plan-template.xlsx
@@ -67,25 +67,25 @@
       <style:table-row-properties style:row-height="9.86mm" fo:break-before="auto" style:use-optimal-row-height="false"/>
     </style:style>
     <style:style style:name="ro8" style:family="table-row">
-      <style:table-row-properties style:row-height="41.01mm" fo:break-before="auto" style:use-optimal-row-height="true"/>
+      <style:table-row-properties style:row-height="76.06mm" fo:break-before="auto" style:use-optimal-row-height="true"/>
     </style:style>
     <style:style style:name="ro9" style:family="table-row">
-      <style:table-row-properties style:row-height="55.88mm" fo:break-before="auto" style:use-optimal-row-height="true"/>
+      <style:table-row-properties style:row-height="50.54mm" fo:break-before="auto" style:use-optimal-row-height="true"/>
     </style:style>
     <style:style style:name="ro10" style:family="table-row">
-      <style:table-row-properties style:row-height="15.52mm" fo:break-before="auto" style:use-optimal-row-height="true"/>
+      <style:table-row-properties style:row-height="15.86mm" fo:break-before="auto" style:use-optimal-row-height="true"/>
     </style:style>
     <style:style style:name="ro11" style:family="table-row">
       <style:table-row-properties style:row-height="5.61mm" fo:break-before="auto" style:use-optimal-row-height="true"/>
     </style:style>
     <style:style style:name="ro12" style:family="table-row">
+      <style:table-row-properties style:row-height="25.79mm" fo:break-before="auto" style:use-optimal-row-height="true"/>
+    </style:style>
+    <style:style style:name="ro13" style:family="table-row">
+      <style:table-row-properties style:row-height="15.52mm" fo:break-before="auto" style:use-optimal-row-height="true"/>
+    </style:style>
+    <style:style style:name="ro14" style:family="table-row">
       <style:table-row-properties style:row-height="25.52mm" fo:break-before="auto" style:use-optimal-row-height="true"/>
-    </style:style>
-    <style:style style:name="ro13" style:family="table-row">
-      <style:table-row-properties style:row-height="10.53mm" fo:break-before="auto" style:use-optimal-row-height="true"/>
-    </style:style>
-    <style:style style:name="ro14" style:family="table-row">
-      <style:table-row-properties style:row-height="25.79mm" fo:break-before="auto" style:use-optimal-row-height="true"/>
     </style:style>
     <style:style style:name="ro15" style:family="table-row">
       <style:table-row-properties style:row-height="21.96mm" fo:break-before="auto" style:use-optimal-row-height="false"/>
@@ -171,7 +171,7 @@
       <style:paragraph-properties css3t:text-justify="auto" fo:margin-left="0mm" style:writing-mode="page"/>
       <style:text-properties fo:color="#000000" style:font-name="Calibri1" fo:font-size="14pt" fo:font-weight="bold" style:font-size-asian="14pt" style:font-weight-asian="bold" style:font-name-complex="Calibri1" style:font-size-complex="14pt" style:font-weight-complex="bold"/>
     </style:style>
-    <style:style style:name="ce27" style:family="table-cell" style:parent-style-name="Excel_20_Built-in_20_Hyperlink">
+    <style:style style:name="ce12" style:family="table-cell" style:parent-style-name="Excel_20_Built-in_20_Hyperlink">
       <style:table-cell-properties fo:background-color="#fac090" style:cell-protect="protected" style:print-content="true" style:diagonal-bl-tr="none" style:diagonal-tl-br="none" style:text-align-source="fix" style:repeat-content="false" fo:wrap-option="wrap" fo:border="none" style:direction="ltr" style:rotation-angle="0" style:rotation-align="none" style:shrink-to-fit="false" style:vertical-align="top" loext:vertical-justify="auto"/>
       <style:paragraph-properties fo:text-align="center" css3t:text-justify="auto" fo:margin-left="0mm" style:writing-mode="page"/>
       <style:text-properties fo:color="#0000ff" style:text-outline="false" style:text-line-through-style="none" style:text-line-through-type="none" style:font-name="Calibri1" fo:font-size="28pt" fo:font-style="normal" fo:text-shadow="none" style:text-underline-style="solid" style:text-underline-width="auto" style:text-underline-color="font-color" fo:font-weight="normal" style:font-size-asian="28pt" style:font-style-asian="normal" style:font-weight-asian="normal" style:font-name-complex="Calibri1" style:font-size-complex="28pt" style:font-style-complex="normal" style:font-weight-complex="normal"/>
@@ -281,6 +281,12 @@
     </style:style>
     <style:style style:name="T1" style:family="text">
       <style:text-properties fo:color="#000000" style:font-name="Calibri" fo:font-size="12pt" fo:font-weight="normal" style:text-underline-style="none" style:text-underline-color="font-color" style:text-line-through-type="none" fo:font-style="normal" style:text-outline="false" fo:text-shadow="none" style:text-line-through-mode="continuous" fo:language="en" fo:country="IN" style:language-asian="zh" style:country-asian="CN" style:language-complex="hi" style:country-complex="IN" style:font-name-asian="Noto Sans CJK SC Regular" style:font-name-complex="Calibri" style:font-size-asian="12pt" style:font-size-complex="12pt" style:font-weight-asian="normal" style:font-weight-complex="normal" style:font-style-asian="normal" style:font-style-complex="normal" style:text-emphasize="none" style:font-relief="none" style:text-overline-style="none" style:text-overline-color="font-color"/>
+    </style:style>
+    <style:style style:name="T2" style:family="text">
+      <style:text-properties fo:font-weight="bold" style:font-weight-asian="bold" style:font-weight-complex="bold"/>
+    </style:style>
+    <style:style style:name="T3" style:family="text">
+      <style:text-properties style:language-complex="hi" style:country-complex="IN" style:text-overline-style="none" style:text-overline-color="font-color" style:font-relief="none" style:text-emphasize="none" style:font-style-complex="normal" style:font-style-asian="normal" style:font-weight-complex="normal" style:font-weight-asian="normal" style:font-size-complex="12pt" style:font-size-asian="12pt" style:font-name-complex="Calibri" style:font-name-asian="Noto Sans CJK SC Regular" fo:color="#000000" style:language-asian="zh" style:country-asian="CN" fo:language="en" fo:country="IN" style:text-line-through-mode="continuous" fo:text-shadow="none" style:text-outline="false" fo:font-style="normal" style:text-line-through-type="none" style:text-underline-style="none" style:text-underline-color="font-color" fo:font-weight="normal" fo:font-size="12pt" style:font-name="Calibri"/>
     </style:style>
   </office:automatic-styles>
   <office:body>
@@ -431,7 +437,36 @@
             <text:p>The web page should display all the fileds</text:p>
             <text:p>Name, date of birth, address, employment type, employer name, salary, EMI(if any),email id, gender, purpose of loan(currently only personal loan) </text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce21" table:number-columns-repeated="2"/>
+          <table:table-cell table:style-name="ce21" office:value-type="string" calcext:value-type="string">
+            <text:p>First Name, Last Name, Date of Birth, Email, Phone, Employment Type</text:p>
+            <text:p>
+              <text:span text:style-name="T2">Salaried:</text:span>
+            </text:p>
+            <text:p>Overall Experience</text:p>
+            <text:p>Experience in Current Comapny</text:p>
+            <text:p>Income Per Month</text:p>
+            <text:p>EMI per Month</text:p>
+            <text:p/>
+            <text:p>
+              <text:span text:style-name="T2">Self Employed:</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">Overall Experience</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">Income Per Annum</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">EMI per Month</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T3">Own Office</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">Own Residence</text:span>
+            </text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce21"/>
           <table:table-cell table:style-name="ce7" table:number-columns-repeated="15"/>
           <table:table-cell table:number-columns-repeated="1003"/>
         </table:table-row>
@@ -444,14 +479,33 @@
             <text:p>Validate the fields</text:p>
           </table:table-cell>
           <table:table-cell table:style-name="ce45" office:value-type="string" calcext:value-type="string">
-            <text:p>Name : Should contain only alphabet and spaces. Special characters, numbers should not be allowed.</text:p>
+            <text:p>Name : Should contain only alphabet. Special characters, numbers should not be allowed.</text:p>
             <text:p/>
             <text:p>Mobile No: Allow only numbers of 10 digit length.</text:p>
             <text:p/>
             <text:p>Email id: Should have proper email format.</text:p>
             <text:p/>
           </table:table-cell>
-          <table:table-cell table:style-name="ce45" table:number-columns-repeated="2"/>
+          <table:table-cell table:style-name="ce45" office:value-type="string" calcext:value-type="string">
+            <text:p>
+              <text:span text:style-name="T1">Name : Allows only alphabet</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1"/>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">Mobile No: Allows only numbers of 10 digit length.</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1"/>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">Email id: Allows only email pattern</text:span>
+            </text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce45" office:value-type="string" calcext:value-type="string">
+            <text:p>Pass</text:p>
+          </table:table-cell>
           <table:table-cell table:style-name="ce7" table:number-columns-repeated="15"/>
           <table:table-cell table:number-columns-repeated="1003"/>
         </table:table-row>
@@ -466,7 +520,12 @@
           <table:table-cell table:style-name="ce45" office:value-type="string" calcext:value-type="string">
             <text:p>Submit button should be disabled and prompt the user to type the particular invalid detail</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce45" table:number-columns-repeated="2"/>
+          <table:table-cell table:style-name="ce45" office:value-type="string" calcext:value-type="string">
+            <text:p>Submit button is disabled</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce45" office:value-type="string" calcext:value-type="string">
+            <text:p>Pass</text:p>
+          </table:table-cell>
           <table:table-cell table:style-name="ce7" table:number-columns-repeated="15"/>
           <table:table-cell table:number-columns-repeated="1003"/>
         </table:table-row>
@@ -481,7 +540,12 @@
           <table:table-cell table:style-name="ce45" office:value-type="string" calcext:value-type="string">
             <text:p>Enable the submit button</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce45" table:number-columns-repeated="2"/>
+          <table:table-cell table:style-name="ce45" office:value-type="string" calcext:value-type="string">
+            <text:p>Submit button is enabled</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce45" office:value-type="string" calcext:value-type="string">
+            <text:p>Pass</text:p>
+          </table:table-cell>
           <table:table-cell table:style-name="ce7" table:number-columns-repeated="15"/>
           <table:table-cell table:number-columns-repeated="1003"/>
         </table:table-row>
@@ -496,7 +560,12 @@
           <table:table-cell table:style-name="ce45" office:value-type="string" calcext:value-type="string">
             <text:p>Calculate and display Eligible loan amount, ROI, Tenure to the eligible Customer. Display the ineligile status to the ineligible Customer</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce45" table:number-columns-repeated="2"/>
+          <table:table-cell table:style-name="ce45" office:value-type="string" calcext:value-type="string">
+            <text:p>Gives the eligibility details.Displays ineligibility to customer</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce45" office:value-type="string" calcext:value-type="string">
+            <text:p>Pass</text:p>
+          </table:table-cell>
           <table:table-cell table:style-name="ce7" table:number-columns-repeated="15"/>
           <table:table-cell table:number-columns-repeated="1003"/>
         </table:table-row>
@@ -511,11 +580,14 @@
           <table:table-cell table:style-name="ce45" office:value-type="string" calcext:value-type="string">
             <text:p>Enable the ‘Upload Documents’ button if the user is eligible</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce45" table:number-columns-repeated="2"/>
-          <table:table-cell table:style-name="ce7" table:number-columns-repeated="15"/>
-          <table:table-cell table:number-columns-repeated="1003"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro13">
+          <table:table-cell table:style-name="ce45" office:value-type="string" calcext:value-type="string">
+            <text:p>Upload Documents is always enabled ass it comes in the eligible form</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce45"/>
+          <table:table-cell table:style-name="ce7" table:number-columns-repeated="15"/>
+          <table:table-cell table:number-columns-repeated="1003"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro10">
           <table:table-cell table:style-name="ce21" office:value-type="float" office:value="7" calcext:value-type="float">
             <text:p>7</text:p>
           </table:table-cell>
@@ -526,7 +598,10 @@
           <table:table-cell table:style-name="ce45" office:value-type="string" calcext:value-type="string">
             <text:p>Disable the ‘Upload Documents’ button</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce45" table:number-columns-repeated="2"/>
+          <table:table-cell table:style-name="ce45" office:value-type="string" calcext:value-type="string">
+            <text:p>Upload Documents is always enabled ass it comes in the eligible form</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce45"/>
           <table:table-cell table:style-name="ce7" table:number-columns-repeated="15"/>
           <table:table-cell table:number-columns-repeated="1003"/>
         </table:table-row>
@@ -541,7 +616,12 @@
           <table:table-cell table:style-name="ce45" office:value-type="string" calcext:value-type="string">
             <text:p>The web page redirects to another page where the user has to enter PAN details and upload documents for verification in given file format.</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce45" table:number-columns-repeated="2"/>
+          <table:table-cell table:style-name="ce45" office:value-type="string" calcext:value-type="string">
+            <text:p>Redirects to new page</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce45" office:value-type="string" calcext:value-type="string">
+            <text:p>pass</text:p>
+          </table:table-cell>
           <table:table-cell table:style-name="ce7" table:number-columns-repeated="15"/>
           <table:table-cell table:number-columns-repeated="1003"/>
         </table:table-row>
@@ -692,30 +772,30 @@
           <table:table-cell table:number-columns-repeated="1003"/>
         </table:table-row>
         <table:table-row table:style-name="ro22">
-          <table:table-cell table:style-name="ce27" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="6" table:number-rows-spanned="4">
+          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="6" table:number-rows-spanned="4">
             <text:p>
               <text:a xlink:href="https://www.smartsheet.com/try-it?trp=8561&amp;utm_source=integrated+content&amp;utm_campaign=/best-agile-pm-templates&amp;utm_medium=agile+test+log+template&amp;lx=Y-edauMi8Lq_ofXZ0cj_JA" xlink:type="simple">Create a Test Plan in Smartsheet</text:a>
             </text:p>
           </table:table-cell>
-          <table:covered-table-cell table:number-columns-repeated="5" table:style-name="ce27"/>
+          <table:covered-table-cell table:number-columns-repeated="5" table:style-name="ce12"/>
           <table:table-cell table:style-name="ce58"/>
           <table:table-cell table:style-name="ce7" table:number-columns-repeated="14"/>
           <table:table-cell table:number-columns-repeated="1003"/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
-          <table:covered-table-cell table:number-columns-repeated="6" table:style-name="ce27"/>
+          <table:covered-table-cell table:number-columns-repeated="6" table:style-name="ce12"/>
           <table:table-cell table:style-name="ce58"/>
           <table:table-cell table:style-name="ce7" table:number-columns-repeated="14"/>
           <table:table-cell table:number-columns-repeated="1003"/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
-          <table:covered-table-cell table:number-columns-repeated="6" table:style-name="ce27"/>
+          <table:covered-table-cell table:number-columns-repeated="6" table:style-name="ce12"/>
           <table:table-cell table:style-name="ce58"/>
           <table:table-cell table:style-name="ce7" table:number-columns-repeated="14"/>
           <table:table-cell table:number-columns-repeated="1003"/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
-          <table:covered-table-cell table:number-columns-repeated="6" table:style-name="ce27"/>
+          <table:covered-table-cell table:number-columns-repeated="6" table:style-name="ce12"/>
           <table:table-cell table:style-name="ce58"/>
           <table:table-cell table:style-name="ce7" table:number-columns-repeated="14"/>
           <table:table-cell table:number-columns-repeated="1003"/>
@@ -726,7 +806,7 @@
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell table:style-name="ce7">
-            <draw:frame table:end-cell-address="Sheet1.G68" table:end-x="16.29mm" table:end-y="4.15mm" draw:z-index="0" draw:name="Picture 2" draw:style-name="gr1" draw:text-style-name="P1" svg:width="360.08mm" svg:height="135.08mm" svg:x="3.18mm" svg:y="1.38mm">
+            <draw:frame table:end-cell-address="Sheet1.G68" table:end-x="16.29mm" table:end-y="4.15mm" draw:z-index="0" draw:name="Picture 2" draw:style-name="gr1" draw:text-style-name="P1" svg:width="360.08mm" svg:height="135.07mm" svg:x="3.18mm" svg:y="1.38mm">
               <draw:image xlink:href="Pictures/100000000000033700000186D4EE65419EDAEED4.png" xlink:type="simple" xlink:show="embed" xlink:actuate="onLoad">
                 <text:p/>
               </draw:image>
@@ -860,11 +940,11 @@
     <meta:creation-date>2016-02-09T21:44:44</meta:creation-date>
     <meta:initial-creator>Emily Esposito</meta:initial-creator>
     <dc:language>en-IN</dc:language>
-    <dc:date>2019-02-21T16:47:41.348058583</dc:date>
-    <meta:editing-cycles>36</meta:editing-cycles>
-    <meta:editing-duration>PT3H22M</meta:editing-duration>
+    <dc:date>2019-03-19T07:39:55.555172202</dc:date>
+    <meta:editing-cycles>37</meta:editing-cycles>
+    <meta:editing-duration>PT3H30M11S</meta:editing-duration>
     <meta:generator>LibreOffice/6.0.3.2$Linux_X86_64 LibreOffice_project/00m0$Build-2</meta:generator>
-    <meta:document-statistic meta:table-count="2" meta:cell-count="84" meta:object-count="1"/>
+    <meta:document-statistic meta:table-count="2" meta:cell-count="97" meta:object-count="1"/>
     <meta:user-defined meta:name="AppVersion">15.0300</meta:user-defined>
     <meta:user-defined meta:name="DocSecurity" meta:value-type="float">0</meta:user-defined>
     <meta:user-defined meta:name="HyperlinksChanged" meta:value-type="boolean">false</meta:user-defined>
@@ -882,14 +962,14 @@
       <config:config-item config:name="VisibleAreaTop" config:type="int">529</config:config-item>
       <config:config-item config:name="VisibleAreaLeft" config:type="int">0</config:config-item>
       <config:config-item config:name="VisibleAreaWidth" config:type="int">79253</config:config-item>
-      <config:config-item config:name="VisibleAreaHeight" config:type="int">80449</config:config-item>
+      <config:config-item config:name="VisibleAreaHeight" config:type="int">84485</config:config-item>
       <config:config-item-map-indexed config:name="Views">
         <config:config-item-map-entry>
           <config:config-item config:name="ViewId" config:type="string">view1</config:config-item>
           <config:config-item-map-named config:name="Tables">
             <config:config-item-map-entry config:name="Sheet1">
               <config:config-item config:name="CursorPositionX" config:type="int">0</config:config-item>
-              <config:config-item config:name="CursorPositionY" config:type="int">19</config:config-item>
+              <config:config-item config:name="CursorPositionY" config:type="int">10</config:config-item>
               <config:config-item config:name="HorizontalSplitMode" config:type="short">0</config:config-item>
               <config:config-item config:name="VerticalSplitMode" config:type="short">0</config:config-item>
               <config:config-item config:name="HorizontalSplitPosition" config:type="int">0</config:config-item>
@@ -898,7 +978,7 @@
               <config:config-item config:name="PositionLeft" config:type="int">0</config:config-item>
               <config:config-item config:name="PositionRight" config:type="int">0</config:config-item>
               <config:config-item config:name="PositionTop" config:type="int">13</config:config-item>
-              <config:config-item config:name="PositionBottom" config:type="int">12</config:config-item>
+              <config:config-item config:name="PositionBottom" config:type="int">10</config:config-item>
               <config:config-item config:name="ZoomType" config:type="short">0</config:config-item>
               <config:config-item config:name="ZoomValue" config:type="int">80</config:config-item>
               <config:config-item config:name="PageViewZoomValue" config:type="int">60</config:config-item>
@@ -957,8 +1037,8 @@
       <config:config-item config:name="IsKernAsianPunctuation" config:type="boolean">false</config:config-item>
       <config:config-item config:name="CharacterCompressionType" config:type="short">0</config:config-item>
       <config:config-item config:name="ApplyUserData" config:type="boolean">true</config:config-item>
-      <config:config-item config:name="PrinterSetup" config:type="base64Binary">kQH+/0dlbmVyaWMgUHJpbnRlcgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAU0dFTlBSVAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAWAAMAsgAAAAAAAAAEAAhSAAAEdAAASm9iRGF0YSAxCnByaW50ZXI9R2VuZXJpYyBQcmludGVyCm9yaWVudGF0aW9uPVBvcnRyYWl0CmNvcGllcz0xCm1hcmdpbmRhanVzdG1lbnQ9MCwwLDAsMApjb2xvcmRlcHRoPTI0CnBzbGV2ZWw9MApwZGZkZXZpY2U9MApjb2xvcmRldmljZT0wClBQRENvbnRleERhdGEKUGFnZVNpemU6QTQARHVwbGV4Ok5vbmUAABIAQ09NUEFUX0RVUExFWF9NT0RFDwBEdXBsZXhNb2RlOjpPZmY=</config:config-item>
-      <config:config-item config:name="PrinterName" config:type="string">Generic Printer</config:config-item>
+      <config:config-item config:name="PrinterSetup" config:type="base64Binary">qQH+/1NhbXN1bmdfTUxfMTY3MF9TZXJpZXNfMTBfNV8wXzIxMgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAQ1VQUzpTYW1zdW5nX01MXzE2NzBfU2VyaWVzXzEwXwAWAAMAxgAAAAAAAAAEAAhSAAAEdAAASm9iRGF0YSAxCnByaW50ZXI9U2Ftc3VuZ19NTF8xNjcwX1Nlcmllc18xMF81XzBfMjEyCm9yaWVudGF0aW9uPVBvcnRyYWl0CmNvcGllcz0xCmNvbGxhdGU9ZmFsc2UKbWFyZ2luZGFqdXN0bWVudD0wLDAsMCwwCmNvbG9yZGVwdGg9MjQKcHNsZXZlbD0wCnBkZmRldmljZT0xCmNvbG9yZGV2aWNlPTAKUFBEQ29udGV4RGF0YQpQYWdlU2l6ZTpBNAAAEgBDT01QQVRfRFVQTEVYX01PREUTAER1cGxleE1vZGU6OlVua25vd24=</config:config-item>
+      <config:config-item config:name="PrinterName" config:type="string">Samsung_ML_1670_Series_10_5_0_212</config:config-item>
       <config:config-item-map-indexed config:name="ForbiddenCharacters">
         <config:config-item-map-entry>
           <config:config-item config:name="Language" config:type="string">en</config:config-item>
@@ -1259,9 +1339,9 @@
         </style:region-left>
         <style:region-right>
           <text:p>
-            <text:date style:data-style-name="N2" text:date-value="2019-02-21">00/00/0000</text:date>
+            <text:date style:data-style-name="N2" text:date-value="2019-03-19">00/00/0000</text:date>
             , 
-            <text:time style:data-style-name="N2" text:time-value="15:55:13.396962999">00:00:00</text:time>
+            <text:time style:data-style-name="N2" text:time-value="06:40:58.869312233">00:00:00</text:time>
           </text:p>
         </style:region-right>
       </style:header>

</xml_diff>